<commit_message>
added all the variables for the analysis with the extra wrangling. applied the odd ratio calculation to the plasma script
</commit_message>
<xml_diff>
--- a/exports/fisher_late_vs_early.xlsx
+++ b/exports/fisher_late_vs_early.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,55 +365,105 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Estado de la Enfermedad al Momento de la Infeccion por SARS-CoV2</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Neumonia</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Antecedente de Trasplante de CPH</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Neutropenia</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>HIPOGAMA</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Dexametasona</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Coinfeccion</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO TRASPLANTE EST AUTOLOGO 1 ALOGENICO 2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Metilprednisolona</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>canula 02 en infusion</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Quimioterapia</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Estado de la Enfermedad al Momento de la Infeccion por SARS-CoV2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Neumonia</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Antecedente de Trasplante de CPH</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>EPOC</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Obesidad</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>HTA</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>DIABETES</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>UTI</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>ARM</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Evolucion</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Viral</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Bacteriana</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>late_vs_early</t>
         </is>
@@ -424,38 +474,68 @@
         <v>0.504839963084693</v>
       </c>
       <c r="B2">
+        <v>1.272238042020146</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Inf</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.2745247695715559</v>
+      </c>
+      <c r="E2">
+        <v>0.1814095767956901</v>
+      </c>
+      <c r="F2">
+        <v>0.5144547528977091</v>
+      </c>
+      <c r="G2">
+        <v>3.997566516229475</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>8.592200908073556</v>
+      </c>
+      <c r="L2">
         <v>0.1106897013394808</v>
       </c>
-      <c r="C2">
-        <v>1.272238042020146</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
-      </c>
-      <c r="E2">
-        <v>0.2745247695715559</v>
-      </c>
-      <c r="F2">
+      <c r="M2">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="N2">
         <v>1.211988842045695</v>
       </c>
-      <c r="H2">
+      <c r="O2">
         <v>0.3711307349059412</v>
       </c>
-      <c r="I2">
+      <c r="P2">
         <v>2.560109292632742</v>
       </c>
-      <c r="J2">
+      <c r="Q2">
         <v>4.283007771697678</v>
       </c>
-      <c r="K2">
+      <c r="R2">
         <v>9.034264144710621</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="S2">
+        <v>6.32070314364931</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>2.585674341544396</v>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>OR</t>
         </is>
@@ -466,36 +546,66 @@
         <v>0.4441883160586889</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.09834368530020698</v>
+      </c>
+      <c r="D3">
+        <v>0.2107955310270561</v>
+      </c>
+      <c r="E3">
+        <v>0.09953271926619613</v>
+      </c>
+      <c r="F3">
+        <v>0.6493952271984307</v>
+      </c>
+      <c r="G3">
+        <v>0.1228006076572503</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.03274330327096515</v>
+      </c>
+      <c r="L3">
         <v>0.06080418437397842</v>
       </c>
-      <c r="C3">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>0.09834368530020698</v>
-      </c>
-      <c r="E3">
-        <v>0.2107955310270561</v>
-      </c>
-      <c r="F3">
+      <c r="N3">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="O3">
+        <v>0.3864416475972541</v>
+      </c>
+      <c r="P3">
+        <v>0.5760869565217393</v>
+      </c>
+      <c r="Q3">
+        <v>0.1819221967963386</v>
+      </c>
+      <c r="R3">
+        <v>0.06080418437397842</v>
+      </c>
+      <c r="S3">
+        <v>0.142080745341615</v>
+      </c>
+      <c r="T3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0.9999999999999999</v>
-      </c>
-      <c r="H3">
-        <v>0.3864416475972541</v>
-      </c>
-      <c r="I3">
-        <v>0.5760869565217393</v>
-      </c>
-      <c r="J3">
-        <v>0.1819221967963386</v>
-      </c>
-      <c r="K3">
-        <v>0.06080418437397842</v>
-      </c>
-      <c r="L3" t="inlineStr">
+      <c r="U3">
+        <v>0.4080966482702923</v>
+      </c>
+      <c r="V3" t="inlineStr">
         <is>
           <t>p</t>
         </is>

</xml_diff>